<commit_message>
Update wordplay_seeds to remove duplicate seeds for different wordplay types
</commit_message>
<xml_diff>
--- a/indicator_clustering/data/wordplay_seeds.xlsx
+++ b/indicator_clustering/data/wordplay_seeds.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="321">
   <si>
     <t>anagram</t>
   </si>
@@ -833,142 +833,151 @@
     <t>wordplay_list</t>
   </si>
   <si>
+    <t>surrounding</t>
+  </si>
+  <si>
+    <t>['container', 'hidden', 'insertion']</t>
+  </si>
+  <si>
+    <t>missing</t>
+  </si>
+  <si>
+    <t>['deletion']</t>
+  </si>
+  <si>
+    <t>assimilating</t>
+  </si>
+  <si>
+    <t>audible</t>
+  </si>
+  <si>
+    <t>aloud</t>
+  </si>
+  <si>
+    <t>['homophone']</t>
+  </si>
+  <si>
     <t>alternating</t>
   </si>
   <si>
     <t>['alternation']</t>
   </si>
   <si>
+    <t>['reversal']</t>
+  </si>
+  <si>
+    <t>disorder</t>
+  </si>
+  <si>
+    <t>['anagram']</t>
+  </si>
+  <si>
+    <t>say</t>
+  </si>
+  <si>
+    <t>incorrect</t>
+  </si>
+  <si>
+    <t>hiding</t>
+  </si>
+  <si>
+    <t>consuming</t>
+  </si>
+  <si>
+    <t>cutting</t>
+  </si>
+  <si>
+    <t>dance</t>
+  </si>
+  <si>
+    <t>declare</t>
+  </si>
+  <si>
+    <t>repair</t>
+  </si>
+  <si>
+    <t>disobey</t>
+  </si>
+  <si>
+    <t>revealing</t>
+  </si>
+  <si>
+    <t>dropping</t>
+  </si>
+  <si>
+    <t>evenly</t>
+  </si>
+  <si>
+    <t>flipped</t>
+  </si>
+  <si>
+    <t>hear</t>
+  </si>
+  <si>
+    <t>intermittent</t>
+  </si>
+  <si>
+    <t>jumbled</t>
+  </si>
+  <si>
+    <t>leak</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>subtract</t>
+  </si>
+  <si>
+    <t>listen</t>
+  </si>
+  <si>
+    <t>mirroring</t>
+  </si>
+  <si>
+    <t>mixed up</t>
+  </si>
+  <si>
+    <t>churning</t>
+  </si>
+  <si>
+    <t>naughty</t>
+  </si>
+  <si>
+    <t>north</t>
+  </si>
+  <si>
     <t>occasional</t>
   </si>
   <si>
-    <t>intermittent</t>
+    <t>odd</t>
+  </si>
+  <si>
+    <t>oppose</t>
   </si>
   <si>
     <t>regular</t>
   </si>
   <si>
-    <t>evenly</t>
-  </si>
-  <si>
-    <t>odd</t>
-  </si>
-  <si>
-    <t>incorrect</t>
-  </si>
-  <si>
-    <t>mixed up</t>
-  </si>
-  <si>
-    <t>['anagram']</t>
+    <t>removed</t>
+  </si>
+  <si>
+    <t>whisper</t>
+  </si>
+  <si>
+    <t>speak</t>
+  </si>
+  <si>
+    <t>spoke</t>
+  </si>
+  <si>
+    <t>strange</t>
+  </si>
+  <si>
+    <t>touched</t>
   </si>
   <si>
     <t>wrong</t>
-  </si>
-  <si>
-    <t>strange</t>
-  </si>
-  <si>
-    <t>disorder</t>
-  </si>
-  <si>
-    <t>naughty</t>
-  </si>
-  <si>
-    <t>jumbled</t>
-  </si>
-  <si>
-    <t>disobey</t>
-  </si>
-  <si>
-    <t>touched</t>
-  </si>
-  <si>
-    <t>repair</t>
-  </si>
-  <si>
-    <t>dance</t>
-  </si>
-  <si>
-    <t>removed</t>
-  </si>
-  <si>
-    <t>['deletion']</t>
-  </si>
-  <si>
-    <t>dropping</t>
-  </si>
-  <si>
-    <t>cutting</t>
-  </si>
-  <si>
-    <t>missing</t>
-  </si>
-  <si>
-    <t>subtract</t>
-  </si>
-  <si>
-    <t>leak</t>
-  </si>
-  <si>
-    <t>['reversal']</t>
-  </si>
-  <si>
-    <t>flipped</t>
-  </si>
-  <si>
-    <t>mirroring</t>
-  </si>
-  <si>
-    <t>oppose</t>
-  </si>
-  <si>
-    <t>left</t>
-  </si>
-  <si>
-    <t>north</t>
-  </si>
-  <si>
-    <t>hear</t>
-  </si>
-  <si>
-    <t>listen</t>
-  </si>
-  <si>
-    <t>['homophone']</t>
-  </si>
-  <si>
-    <t>say</t>
-  </si>
-  <si>
-    <t>declare</t>
-  </si>
-  <si>
-    <t>speak</t>
-  </si>
-  <si>
-    <t>spoke</t>
-  </si>
-  <si>
-    <t>audible</t>
-  </si>
-  <si>
-    <t>aloud</t>
-  </si>
-  <si>
-    <t>['container', 'hidden', 'insertion']</t>
-  </si>
-  <si>
-    <t>consuming</t>
-  </si>
-  <si>
-    <t>surrounding</t>
-  </si>
-  <si>
-    <t>revealing</t>
-  </si>
-  <si>
-    <t>hiding</t>
   </si>
 </sst>
 </file>
@@ -1017,7 +1026,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1046,7 +1055,6 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -6183,7 +6191,7 @@
         <v>272</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>272</v>
+        <v>144</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>273</v>
@@ -6194,18 +6202,18 @@
         <v>274</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>179</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>275</v>
+        <v>196</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>273</v>
@@ -6213,10 +6221,10 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>276</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>207</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>273</v>
@@ -6224,10 +6232,10 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>159</v>
+        <v>24</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>277</v>
+        <v>24</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>273</v>
@@ -6235,18 +6243,18 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>136</v>
-      </c>
       <c r="C7" s="3" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>280</v>
@@ -6257,244 +6265,244 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>279</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>279</v>
+        <v>183</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>283</v>
+        <v>11</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>62</v>
+        <v>243</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>285</v>
+        <v>36</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>284</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>287</v>
+        <v>48</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>284</v>
+        <v>32</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>243</v>
+        <v>162</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>238</v>
+        <v>32</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>288</v>
+        <v>216</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>238</v>
+        <v>32</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>30</v>
+        <v>223</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>84</v>
+        <v>137</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>94</v>
+        <v>168</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>153</v>
+        <v>32</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>153</v>
+        <v>229</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>153</v>
+        <v>32</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>130</v>
+        <v>32</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>153</v>
+        <v>238</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>242</v>
+        <v>30</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>153</v>
+        <v>12</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>12</v>
+        <v>153</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>12</v>
+        <v>285</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>26</v>
+        <v>291</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>12</v>
+        <v>292</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>293</v>
+        <v>94</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>12</v>
+        <v>288</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>294</v>
+        <v>47</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>19</v>
+        <v>293</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>295</v>
+        <v>138</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
     </row>
     <row r="31">
@@ -6502,98 +6510,98 @@
         <v>12</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>34</v>
+        <v>295</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>292</v>
+        <v>275</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>66</v>
+        <v>145</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="s">
-        <v>296</v>
+        <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>170</v>
+        <v>239</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
-        <v>12</v>
+        <v>196</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>42</v>
+        <v>211</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="3" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>258</v>
+        <v>84</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="s">
-        <v>183</v>
+        <v>208</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>225</v>
+        <v>56</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>298</v>
+        <v>273</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="3" t="s">
-        <v>183</v>
+        <v>159</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>11</v>
+        <v>296</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>298</v>
+        <v>281</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="3" t="s">
-        <v>183</v>
+        <v>12</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>198</v>
+        <v>26</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>298</v>
+        <v>275</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="3" t="s">
-        <v>165</v>
+        <v>294</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>73</v>
+        <v>161</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>298</v>
+        <v>273</v>
       </c>
     </row>
     <row r="40">
@@ -6601,703 +6609,703 @@
         <v>165</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>298</v>
+        <v>282</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="s">
-        <v>165</v>
+        <v>294</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>300</v>
+        <v>10</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>298</v>
+        <v>273</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>218</v>
+        <v>18</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>298</v>
+        <v>273</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="3" t="s">
-        <v>302</v>
+        <v>208</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>302</v>
+        <v>64</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>298</v>
+        <v>273</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="3" t="s">
-        <v>265</v>
+        <v>196</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>265</v>
+        <v>188</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>298</v>
+        <v>273</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="s">
-        <v>100</v>
+        <v>298</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>102</v>
+        <v>298</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>298</v>
+        <v>279</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="s">
-        <v>100</v>
+        <v>196</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>184</v>
+        <v>72</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>298</v>
+        <v>273</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="s">
-        <v>100</v>
+        <v>287</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>81</v>
+        <v>2</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>298</v>
+        <v>273</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="s">
-        <v>100</v>
+        <v>287</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>95</v>
+        <v>180</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>298</v>
+        <v>273</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="s">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>98</v>
+        <v>196</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>298</v>
+        <v>273</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="s">
-        <v>303</v>
+        <v>196</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>303</v>
+        <v>55</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>298</v>
+        <v>273</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="s">
-        <v>304</v>
+        <v>32</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>305</v>
+        <v>53</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>306</v>
+        <v>273</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="s">
-        <v>304</v>
+        <v>32</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>304</v>
+        <v>17</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>306</v>
+        <v>273</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>221</v>
+        <v>195</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>306</v>
+        <v>281</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="3" t="s">
-        <v>307</v>
+        <v>283</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>52</v>
+        <v>300</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>306</v>
+        <v>284</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>308</v>
+        <v>196</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>306</v>
+        <v>273</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="3" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>309</v>
+        <v>258</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>306</v>
+        <v>275</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>306</v>
+        <v>282</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>36</v>
+        <v>170</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>306</v>
+        <v>275</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="3" t="s">
-        <v>307</v>
+        <v>100</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>232</v>
+        <v>95</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>306</v>
+        <v>282</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="3" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>306</v>
+        <v>279</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="3" t="s">
-        <v>311</v>
+        <v>12</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>306</v>
+        <v>275</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="3" t="s">
-        <v>311</v>
+        <v>208</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>92</v>
+        <v>197</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>306</v>
+        <v>273</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="3" t="s">
-        <v>311</v>
+        <v>285</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>240</v>
+        <v>221</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>306</v>
+        <v>279</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="3" t="s">
-        <v>311</v>
+        <v>165</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>76</v>
+        <v>305</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>306</v>
+        <v>282</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="3" t="s">
-        <v>152</v>
+        <v>274</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>152</v>
+        <v>274</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>306</v>
+        <v>275</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="3" t="s">
-        <v>152</v>
+        <v>286</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>232</v>
+        <v>306</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>306</v>
+        <v>284</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>36</v>
+        <v>307</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>306</v>
+        <v>284</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="3" t="s">
-        <v>32</v>
+        <v>153</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>32</v>
+        <v>153</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>313</v>
+        <v>284</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="3" t="s">
-        <v>32</v>
+        <v>283</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>53</v>
+        <v>308</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>313</v>
+        <v>284</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="3" t="s">
-        <v>314</v>
+        <v>152</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>313</v>
+        <v>279</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="3" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>168</v>
+        <v>309</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>313</v>
+        <v>282</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="3" t="s">
-        <v>314</v>
+        <v>12</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>313</v>
+        <v>275</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="3" t="s">
-        <v>196</v>
+        <v>310</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="3" t="s">
-        <v>196</v>
+        <v>311</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>202</v>
+        <v>136</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="3" t="s">
-        <v>196</v>
+        <v>312</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>313</v>
+        <v>282</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="B76" s="9" t="s">
-        <v>31</v>
+        <v>272</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>187</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>313</v>
+        <v>273</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="B77" s="9" t="s">
-        <v>39</v>
+        <v>277</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>313</v>
+        <v>279</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="3" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>313</v>
+        <v>273</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="3" t="s">
-        <v>315</v>
+        <v>208</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>313</v>
+        <v>273</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>9</v>
+        <v>196</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>313</v>
+        <v>273</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="3" t="s">
-        <v>315</v>
+        <v>100</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>313</v>
+        <v>282</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="3" t="s">
-        <v>24</v>
+        <v>165</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>313</v>
+        <v>282</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="3" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>18</v>
+        <v>207</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="3" t="s">
-        <v>208</v>
+        <v>12</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>17</v>
+        <v>314</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>313</v>
+        <v>275</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="3" t="s">
-        <v>317</v>
+        <v>285</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>48</v>
+        <v>232</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>313</v>
+        <v>279</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="3" t="s">
-        <v>208</v>
+        <v>152</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>56</v>
+        <v>315</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>313</v>
+        <v>279</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="3" t="s">
-        <v>208</v>
+        <v>183</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>64</v>
+        <v>198</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>313</v>
+        <v>282</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="3" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>72</v>
+        <v>225</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>313</v>
+        <v>282</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="3" t="s">
-        <v>208</v>
+        <v>100</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>313</v>
+        <v>282</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="3" t="s">
-        <v>208</v>
+        <v>285</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>313</v>
+        <v>279</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="3" t="s">
-        <v>317</v>
+        <v>208</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>137</v>
+        <v>181</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>313</v>
+        <v>273</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="3" t="s">
-        <v>317</v>
+        <v>208</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>160</v>
+        <v>86</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>313</v>
+        <v>273</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="3" t="s">
-        <v>317</v>
+        <v>287</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>313</v>
+        <v>273</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="3" t="s">
-        <v>317</v>
+        <v>208</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>2</v>
+        <v>163</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>313</v>
+        <v>273</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="3" t="s">
-        <v>316</v>
+        <v>208</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>138</v>
+        <v>208</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>313</v>
+        <v>273</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="3" t="s">
-        <v>316</v>
+        <v>208</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>161</v>
+        <v>217</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>313</v>
+        <v>273</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="3" t="s">
-        <v>316</v>
+        <v>100</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>313</v>
+        <v>282</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="3" t="s">
-        <v>32</v>
+        <v>208</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>139</v>
+        <v>224</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>313</v>
+        <v>273</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="3" t="s">
-        <v>32</v>
+        <v>285</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>162</v>
+        <v>316</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>313</v>
+        <v>279</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="3" t="s">
-        <v>32</v>
+        <v>285</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>17</v>
+        <v>317</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>313</v>
+        <v>279</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="3" t="s">
-        <v>32</v>
+        <v>286</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>196</v>
+        <v>318</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>313</v>
+        <v>284</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="3" t="s">
-        <v>32</v>
+        <v>153</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>167</v>
+        <v>242</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>313</v>
+        <v>284</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="3" t="s">
-        <v>32</v>
+        <v>238</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>216</v>
+        <v>319</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>313</v>
+        <v>284</v>
       </c>
     </row>
     <row r="104">
@@ -7305,147 +7313,101 @@
         <v>32</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>223</v>
+        <v>139</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>313</v>
+        <v>273</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="3" t="s">
-        <v>32</v>
+        <v>286</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>229</v>
+        <v>62</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>313</v>
+        <v>284</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="3" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>234</v>
+        <v>102</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>313</v>
+        <v>282</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="3" t="s">
-        <v>32</v>
+        <v>277</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>313</v>
+        <v>279</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="3" t="s">
-        <v>208</v>
+        <v>277</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>140</v>
+        <v>92</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>313</v>
+        <v>279</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="3" t="s">
-        <v>208</v>
+        <v>265</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>163</v>
+        <v>265</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>313</v>
+        <v>282</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="3" t="s">
-        <v>208</v>
+        <v>32</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>313</v>
+        <v>273</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="3" t="s">
-        <v>208</v>
+        <v>274</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>197</v>
+        <v>66</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>313</v>
+        <v>275</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="3" t="s">
-        <v>208</v>
+        <v>286</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>208</v>
+        <v>320</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" s="10">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("COUNTUNIQUE(A2:A114)"),34.0)</f>
-        <v>34</v>
-      </c>
-      <c r="B115" s="10">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("COUNTUNIQUE(B2:B114)"),110.0)</f>
-        <v>110</v>
-      </c>
-      <c r="C115" s="10">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("COUNTUNIQUE(C2:C114)"),6.0)</f>
-        <v>6</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFFFFF"/>
-        <color rgb="FF57BB8A"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>